<commit_message>
add translations for student pages in frontend
</commit_message>
<xml_diff>
--- a/frontend/src/translations/TraduccionesMetahospital.xlsx
+++ b/frontend/src/translations/TraduccionesMetahospital.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="703">
   <si>
     <t>Tname</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Eskola</t>
   </si>
   <si>
+    <t>Centre</t>
+  </si>
+  <si>
     <t>Escola</t>
   </si>
   <si>
@@ -88,7 +91,7 @@
     <t>Eskolak</t>
   </si>
   <si>
-    <t>Escoles</t>
+    <t>Centres</t>
   </si>
   <si>
     <t>Escolas</t>
@@ -202,7 +205,7 @@
     <t>Ikaslea</t>
   </si>
   <si>
-    <t>Estudiant</t>
+    <t>Alumne/a</t>
   </si>
   <si>
     <t>student_p</t>
@@ -217,7 +220,7 @@
     <t>Ikasleak</t>
   </si>
   <si>
-    <t>Estudiants</t>
+    <t>Alumnes</t>
   </si>
   <si>
     <t>Estudantes</t>
@@ -229,30 +232,36 @@
     <t>Teacher</t>
   </si>
   <si>
+    <t>Profesor/a</t>
+  </si>
+  <si>
+    <t>Irakaslea</t>
+  </si>
+  <si>
+    <t>Professor/a</t>
+  </si>
+  <si>
     <t>Profesor</t>
   </si>
   <si>
-    <t>Irakaslea</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
     <t>teacher_p</t>
   </si>
   <si>
     <t>Teachers</t>
   </si>
   <si>
+    <t>Profesores/as</t>
+  </si>
+  <si>
+    <t>Irakasleak</t>
+  </si>
+  <si>
+    <t>Professors</t>
+  </si>
+  <si>
     <t>Profesores</t>
   </si>
   <si>
-    <t>Irakasleak</t>
-  </si>
-  <si>
-    <t>Professors</t>
-  </si>
-  <si>
     <t>admin_s</t>
   </si>
   <si>
@@ -508,7 +517,7 @@
     <t>Hautatu Eskola</t>
   </si>
   <si>
-    <t>Seleccionar Escola</t>
+    <t>Seleccionar centre</t>
   </si>
   <si>
     <t>Seleccione Escola</t>
@@ -568,13 +577,13 @@
     <t>Teacher's name</t>
   </si>
   <si>
-    <t>Nombre del Profesor</t>
+    <t>Nombre del Profesor/a</t>
   </si>
   <si>
     <t>Irakaslearen izena</t>
   </si>
   <si>
-    <t>Nom del Professor</t>
+    <t>Nom del professor/a</t>
   </si>
   <si>
     <t>Nome do profesor</t>
@@ -592,7 +601,7 @@
     <t>Ikaslearen izena</t>
   </si>
   <si>
-    <t>Nom de l'Estudiant</t>
+    <t>Nom de l'alumne/a</t>
   </si>
   <si>
     <t>Nome do alumno</t>
@@ -655,7 +664,7 @@
     <t>Nire ikasleak</t>
   </si>
   <si>
-    <t>Els meus Estudiants</t>
+    <t>El meu alumnat</t>
   </si>
   <si>
     <t>Os meus alumnos</t>
@@ -673,7 +682,7 @@
     <t>Kodea</t>
   </si>
   <si>
-    <t>Codi</t>
+    <t>Còdic</t>
   </si>
   <si>
     <t>case_select</t>
@@ -706,7 +715,7 @@
     <t>Aukeratu ikasleak</t>
   </si>
   <si>
-    <t>Selecciona alumnes</t>
+    <t>Selecciona alumnat</t>
   </si>
   <si>
     <t>Seleccionar alumnos</t>
@@ -778,7 +787,7 @@
     <t>Autentifikazio-kodea</t>
   </si>
   <si>
-    <t>Codi d'autenticació</t>
+    <t>Còdic d'autentificació</t>
   </si>
   <si>
     <t>Código de autenticación</t>
@@ -814,7 +823,7 @@
     <t>Aldatu pasahitza</t>
   </si>
   <si>
-    <t>Canvia contrasenya</t>
+    <t>Canviar contrasenya</t>
   </si>
   <si>
     <t>Cambie o contrasinal</t>
@@ -862,7 +871,7 @@
     <t>Ziur ezabatu nahi duzula?</t>
   </si>
   <si>
-    <t>Segur que vols eliminar?</t>
+    <t>Estàs segur que vols eleminiar?</t>
   </si>
   <si>
     <t>Estás seguro de que queres eliminar?</t>
@@ -925,9 +934,6 @@
     <t>Utzi</t>
   </si>
   <si>
-    <t>Cancel·la</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -940,9 +946,6 @@
     <t>Aukeratu eskola bat</t>
   </si>
   <si>
-    <t>Selecciona una escola</t>
-  </si>
-  <si>
     <t>Selecciona unha escola</t>
   </si>
   <si>
@@ -1096,7 +1099,7 @@
     <t>Behar bezala eguneratu da eskola</t>
   </si>
   <si>
-    <t>Escola actualitzada correctament</t>
+    <t>Centre actualitzat correctament</t>
   </si>
   <si>
     <t>Actualizouse a escola correctamente</t>
@@ -1114,7 +1117,7 @@
     <t>Eskola ondo gehitu da</t>
   </si>
   <si>
-    <t>Escola agregada correctament</t>
+    <t>Centre afegit correctament</t>
   </si>
   <si>
     <t>Engadiuse a escola correctamente</t>
@@ -1165,7 +1168,7 @@
     <t>Behar bezala ezabatu da taldea</t>
   </si>
   <si>
-    <t>Grup eliminat correctament</t>
+    <t>Grup afegit correctament</t>
   </si>
   <si>
     <t>O grupo eliminouse correctamente</t>
@@ -1183,7 +1186,7 @@
     <t>Leheneratu pasahitza</t>
   </si>
   <si>
-    <t>Restablir Contrasenya</t>
+    <t>Restablir contrasenya</t>
   </si>
   <si>
     <t>Restaurar contrasinal</t>
@@ -1201,7 +1204,7 @@
     <t>Ziur pasahitza berrezarri nahi duzula?</t>
   </si>
   <si>
-    <t>Esteu segur que voleu restablir Contrasenya?</t>
+    <t>Estàs segur que vols restablir la contrasenya?</t>
   </si>
   <si>
     <t>Estás seguro de que queres restablecer o teu contrasinal?</t>
@@ -1273,7 +1276,7 @@
     <t>Ezin izan dira erabiltzaileak lortu</t>
   </si>
   <si>
-    <t>No s'ha pogut obtenir els usuaris</t>
+    <t>No es pot obtenir als usuaris</t>
   </si>
   <si>
     <t>Non se puideron conseguir usuarios</t>
@@ -1285,13 +1288,13 @@
     <t>School teachers could not be obtained.</t>
   </si>
   <si>
-    <t>No se pudo obtener a los profesores de la escuela</t>
+    <t>No se pudo obtener al profesorado de la escuela</t>
   </si>
   <si>
     <t>Ezin izan dira ikastetxeko irakasleak lortu</t>
   </si>
   <si>
-    <t>No s'ha pogut obtenir els professors de l'escola</t>
+    <t>No es pot obtenir al professorat del centre</t>
   </si>
   <si>
     <t>Non se puido conseguir profesores da escola</t>
@@ -1309,7 +1312,7 @@
     <t>Ezin izan dira ikastetxeko erabiltzaileak lortu</t>
   </si>
   <si>
-    <t>No s'ha pogut obtenir els usuaris de l'escola</t>
+    <t>No es pot obtenir als usuaris del centre</t>
   </si>
   <si>
     <t>Non se puideron conseguir usuarios da escola</t>
@@ -1381,7 +1384,7 @@
     <t>Ezin izan da talderik eguneratu/sortu</t>
   </si>
   <si>
-    <t>No s'ha pogut actualitzar/crear un grup</t>
+    <t>No s'ha pogut crear/actualitzar un grup</t>
   </si>
   <si>
     <t>Non se puido actualizar/crear un grupo</t>
@@ -1399,7 +1402,7 @@
     <t>Ezin izan da behar bezala sortu eskola berria</t>
   </si>
   <si>
-    <t>No s'ha pogut crear correctament la nova escola</t>
+    <t>No s'ha pogut crear correctament el nou centre</t>
   </si>
   <si>
     <t>A nova escola non se puido crear correctamente</t>
@@ -1417,7 +1420,7 @@
     <t>Ezin izan dira eskolarik lortu, saiatu berriro edo saiatu geroago</t>
   </si>
   <si>
-    <t>No es va poder obtenir escoles, intenta-ho de nou o prova més tard</t>
+    <t>No s'ha pogut obtenir centres, intenta-ho de nou o prova més tard</t>
   </si>
   <si>
     <t>Non se puideron obter escolas, téntao de novo ou téntao máis tarde</t>
@@ -1471,6 +1474,9 @@
     <t>Erabiltzaile-izena edo pasahitza zuzena al da?</t>
   </si>
   <si>
+    <t>El nom d'usuari o la contrasenya són correctes?</t>
+  </si>
+  <si>
     <t>O nome de usuario ou contrasinal é correcto?</t>
   </si>
   <si>
@@ -1504,7 +1510,7 @@
     <t>Ezin izan da zerbitzariarekin konexiorik ezarri. Saiatu berriro edo saiatu berriro geroago</t>
   </si>
   <si>
-    <t>No s'ha pogut establir una connexió amb el servidor, intenta-ho de nou o prova-ho més tard</t>
+    <t>No s´ha pogut establir una connexió amb el servidor, intenta-ho de nou o prova-ho més tard</t>
   </si>
   <si>
     <t>Non se puido establecer unha conexión co servidor. Téntao de novo ou ténteo de novo máis tarde</t>
@@ -1534,13 +1540,13 @@
     <t>It is necessary for students as well as teachers to select School</t>
   </si>
   <si>
-    <t>Es necesario para estudiantes como profesores seleccionar Escuela</t>
+    <t>Es necesario para estudiantes como profesores/as seleccionar "Escuela"</t>
   </si>
   <si>
     <t>Ikasleek irakasle gisa Eskola hautatzea beharrezkoa da</t>
   </si>
   <si>
-    <t>És necessari per a estudiants com a professors seleccionar Escola</t>
+    <t>És necessari que alumnat i professorat seleccionin un centre</t>
   </si>
   <si>
     <t>É necesario que os alumnos como profesores seleccionen Escola</t>
@@ -1639,9 +1645,6 @@
     <t>Ezin izan da ikastaro bat eguneratu/sortu</t>
   </si>
   <si>
-    <t>No s'ha pogut actualitzar/crear un curs</t>
-  </si>
-  <si>
     <t>Non se puido actualizar/crear un curso</t>
   </si>
   <si>
@@ -1681,13 +1684,13 @@
     <t>Teacher successfully created</t>
   </si>
   <si>
-    <t>Profesor creado satisfactoriamente</t>
+    <t>Profesor/a creado satisfactoriamente</t>
   </si>
   <si>
     <t>Irakaslea behar bezala sortu da</t>
   </si>
   <si>
-    <t>Professor creat satisfactòriament</t>
+    <t>Professor/a creat satisfactòriament</t>
   </si>
   <si>
     <t>Creouse correctamente o profesor</t>
@@ -1699,28 +1702,31 @@
     <t>Satisfactorily updated teacher</t>
   </si>
   <si>
+    <t>Profesor/a actualizado satisfactoriamente</t>
+  </si>
+  <si>
+    <t>Irakaslea ongi eguneratua</t>
+  </si>
+  <si>
+    <t>Professor/a actualitzat satisfactòriament</t>
+  </si>
+  <si>
     <t>Profesor actualizado satisfactoriamente</t>
   </si>
   <si>
-    <t>Irakaslea ongi eguneratua</t>
-  </si>
-  <si>
-    <t>Professor actualitzat satisfactòriament</t>
-  </si>
-  <si>
     <t>teacher_update_create_fail</t>
   </si>
   <si>
     <t>Error when deleting/updating teacher</t>
   </si>
   <si>
-    <t>Error al eliminar/actualizar profesor</t>
+    <t>Error al eliminar/actualizar profesor/a</t>
   </si>
   <si>
     <t>Errorea irakaslea ezabatzean/eguneratzean</t>
   </si>
   <si>
-    <t>Error en eliminar/actualitzar professor</t>
+    <t>Error en eliminar/actualitzar professor/a</t>
   </si>
   <si>
     <t>Produciuse un erro ao eliminar/actualizar o profesor</t>
@@ -1732,13 +1738,13 @@
     <t>Teacher successfully eliminated</t>
   </si>
   <si>
-    <t>Profesor eliminado satisfactoriamente</t>
+    <t>Profesor/a eliminado satisfactoriamente</t>
   </si>
   <si>
     <t>Irakaslea arrakastaz kanporatua</t>
   </si>
   <si>
-    <t>Professor eliminat satisfactòriament</t>
+    <t>Professor/a eliminat satisfactòriament</t>
   </si>
   <si>
     <t>Profesor eliminado con éxito</t>
@@ -1750,13 +1756,13 @@
     <t>Error when deleting teacher</t>
   </si>
   <si>
-    <t>Error al eliminar profesor</t>
+    <t>Error al eliminar profesor/a</t>
   </si>
   <si>
     <t>Errore bat gertatu da irakaslea ezabatzean</t>
   </si>
   <si>
-    <t>Error en eliminar professor</t>
+    <t>Error en eliminar professor/a</t>
   </si>
   <si>
     <t>Produciuse un erro ao eliminar o profesor</t>
@@ -1852,10 +1858,7 @@
     <t>Produciuse un erro ao eliminar o alumno</t>
   </si>
   <si>
-    <t>Nombre del profesor</t>
-  </si>
-  <si>
-    <t>Nom del professor</t>
+    <t>Nombre del profesor/a</t>
   </si>
   <si>
     <t>Student name</t>
@@ -1864,9 +1867,6 @@
     <t>Nombre del estudiante</t>
   </si>
   <si>
-    <t>Nom de l'estudiant</t>
-  </si>
-  <si>
     <t>user_not_found</t>
   </si>
   <si>
@@ -1915,7 +1915,7 @@
     <t>Ez da koderik sortu</t>
   </si>
   <si>
-    <t>No hi ha codi generat</t>
+    <t>No hi ha códic generat</t>
   </si>
   <si>
     <t>Non hai ningún código xerado</t>
@@ -1933,7 +1933,7 @@
     <t>Sortu kodea</t>
   </si>
   <si>
-    <t>Generar codi</t>
+    <t>Generar códic</t>
   </si>
   <si>
     <t>Xerar código</t>
@@ -1960,7 +1960,7 @@
     <t>submit</t>
   </si>
   <si>
-    <t>Confirm</t>
+    <t>Submit</t>
   </si>
   <si>
     <t>Confirmar</t>
@@ -1970,13 +1970,163 @@
   </si>
   <si>
     <t>Confirma</t>
+  </si>
+  <si>
+    <t>my_groups</t>
+  </si>
+  <si>
+    <t>My groups</t>
+  </si>
+  <si>
+    <t>Mis grupos</t>
+  </si>
+  <si>
+    <t>nire taldeak</t>
+  </si>
+  <si>
+    <t>els meus grups</t>
+  </si>
+  <si>
+    <t>meus grupos</t>
+  </si>
+  <si>
+    <t>updating</t>
+  </si>
+  <si>
+    <t>Updating</t>
+  </si>
+  <si>
+    <t>Actualizando</t>
+  </si>
+  <si>
+    <t>Eguneratzea</t>
+  </si>
+  <si>
+    <t>Actualitzant</t>
+  </si>
+  <si>
+    <t>image_update_successful</t>
+  </si>
+  <si>
+    <t>Image successfully updated</t>
+  </si>
+  <si>
+    <t>Imagen actualizada satisfactoriamente</t>
+  </si>
+  <si>
+    <t>Irudia behar bezala eguneratu da</t>
+  </si>
+  <si>
+    <t>Imatge actualitzada satisfactòriament</t>
+  </si>
+  <si>
+    <t>A imaxe actualizouse correctamente</t>
+  </si>
+  <si>
+    <t>user_image</t>
+  </si>
+  <si>
+    <t>Image by user _</t>
+  </si>
+  <si>
+    <t>Imagen del usuario _</t>
+  </si>
+  <si>
+    <t>_ erabiltzailearen irudia</t>
+  </si>
+  <si>
+    <t>Imatge de l'usuari _</t>
+  </si>
+  <si>
+    <t>Imaxe do usuario _</t>
+  </si>
+  <si>
+    <t>go_back</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>Volver</t>
+  </si>
+  <si>
+    <t>Atzera egin</t>
+  </si>
+  <si>
+    <t>Tornar</t>
+  </si>
+  <si>
+    <t>Volve atrás</t>
+  </si>
+  <si>
+    <t>exercise_s</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Ejercicio</t>
+  </si>
+  <si>
+    <t>Ariketa</t>
+  </si>
+  <si>
+    <t>Exercici</t>
+  </si>
+  <si>
+    <t>Exercicio</t>
+  </si>
+  <si>
+    <t>exercise_p</t>
+  </si>
+  <si>
+    <t>Exercises</t>
+  </si>
+  <si>
+    <t>Ejercicios</t>
+  </si>
+  <si>
+    <t>Ariketak</t>
+  </si>
+  <si>
+    <t>Exercicis</t>
+  </si>
+  <si>
+    <t>Exercicios</t>
+  </si>
+  <si>
+    <t>select_filter</t>
+  </si>
+  <si>
+    <t>Select filter</t>
+  </si>
+  <si>
+    <t>Seleccionar filtre</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Calificación</t>
+  </si>
+  <si>
+    <t>Titulazioa</t>
+  </si>
+  <si>
+    <t>Qualificació</t>
+  </si>
+  <si>
+    <t>Cualificación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1993,6 +2143,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2021,7 +2175,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2033,6 +2187,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2254,7 +2417,7 @@
     <col customWidth="1" min="2" max="2" width="32.25"/>
     <col customWidth="1" min="3" max="3" width="29.75"/>
     <col customWidth="1" min="4" max="4" width="23.88"/>
-    <col customWidth="1" min="5" max="5" width="27.5"/>
+    <col customWidth="1" min="5" max="5" width="35.63"/>
     <col customWidth="1" min="6" max="6" width="20.75"/>
   </cols>
   <sheetData>
@@ -2355,11 +2518,11 @@
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -2376,22 +2539,22 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2408,22 +2571,22 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2440,22 +2603,22 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2472,22 +2635,22 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2504,22 +2667,22 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2536,22 +2699,22 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2568,22 +2731,22 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2600,22 +2763,22 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2632,22 +2795,22 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="E13" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2664,22 +2827,22 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2696,22 +2859,22 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2728,22 +2891,22 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2760,22 +2923,22 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2792,22 +2955,22 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2824,22 +2987,22 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2856,22 +3019,22 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2888,22 +3051,22 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2920,22 +3083,22 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2952,22 +3115,22 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2984,22 +3147,22 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -3016,22 +3179,22 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3048,22 +3211,22 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3080,22 +3243,22 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -3112,22 +3275,22 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -3144,22 +3307,22 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3176,22 +3339,22 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -3208,22 +3371,22 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -3240,22 +3403,22 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -3272,22 +3435,22 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -3304,22 +3467,22 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -3336,22 +3499,22 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3368,22 +3531,22 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -3400,22 +3563,22 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -3432,22 +3595,22 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -3464,22 +3627,22 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3496,22 +3659,22 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -3528,22 +3691,22 @@
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3560,22 +3723,22 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -3592,22 +3755,22 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -3624,22 +3787,22 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -3656,22 +3819,22 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -3688,22 +3851,22 @@
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -3720,22 +3883,22 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>258</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3752,22 +3915,22 @@
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -3784,22 +3947,22 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -3816,22 +3979,22 @@
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -3848,22 +4011,22 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3880,22 +4043,22 @@
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>283</v>
+        <v>285</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -3912,22 +4075,22 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3944,22 +4107,22 @@
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -3976,22 +4139,22 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -4008,22 +4171,22 @@
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>304</v>
+        <v>306</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>305</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -4040,22 +4203,22 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -4072,22 +4235,22 @@
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -4104,22 +4267,22 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -4136,22 +4299,22 @@
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="F60" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -4168,22 +4331,22 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -4200,22 +4363,22 @@
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -4232,22 +4395,22 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -4264,22 +4427,22 @@
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D64" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>339</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -4296,22 +4459,22 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -4328,22 +4491,22 @@
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D66" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -4360,22 +4523,22 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -4392,22 +4555,22 @@
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="E68" s="3" t="s">
         <v>361</v>
       </c>
+      <c r="E68" s="5" t="s">
+        <v>362</v>
+      </c>
       <c r="F68" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
@@ -4424,22 +4587,22 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E69" s="2" t="s">
         <v>367</v>
       </c>
+      <c r="E69" s="4" t="s">
+        <v>368</v>
+      </c>
       <c r="F69" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -4456,22 +4619,22 @@
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D70" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>371</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
@@ -4488,22 +4651,22 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -4520,22 +4683,22 @@
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="E72" s="3" t="s">
         <v>384</v>
       </c>
+      <c r="E72" s="5" t="s">
+        <v>385</v>
+      </c>
       <c r="F72" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
@@ -4552,22 +4715,22 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E73" s="2" t="s">
         <v>390</v>
       </c>
+      <c r="E73" s="4" t="s">
+        <v>391</v>
+      </c>
       <c r="F73" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -4584,22 +4747,22 @@
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="E74" s="3" t="s">
         <v>396</v>
       </c>
+      <c r="E74" s="5" t="s">
+        <v>397</v>
+      </c>
       <c r="F74" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -4616,22 +4779,22 @@
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -4648,22 +4811,22 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -4680,22 +4843,22 @@
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
@@ -4712,22 +4875,22 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E78" s="2" t="s">
         <v>420</v>
       </c>
+      <c r="E78" s="4" t="s">
+        <v>421</v>
+      </c>
       <c r="F78" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -4744,22 +4907,22 @@
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E79" s="3" t="s">
         <v>426</v>
       </c>
+      <c r="E79" s="5" t="s">
+        <v>427</v>
+      </c>
       <c r="F79" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -4776,22 +4939,22 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="E80" s="2" t="s">
         <v>432</v>
       </c>
+      <c r="E80" s="4" t="s">
+        <v>433</v>
+      </c>
       <c r="F80" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -4808,22 +4971,22 @@
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
@@ -4840,22 +5003,22 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -4872,22 +5035,22 @@
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="E83" s="3" t="s">
         <v>450</v>
       </c>
+      <c r="E83" s="5" t="s">
+        <v>451</v>
+      </c>
       <c r="F83" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
@@ -4904,22 +5067,22 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="E84" s="2" t="s">
         <v>456</v>
       </c>
+      <c r="E84" s="4" t="s">
+        <v>457</v>
+      </c>
       <c r="F84" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -4936,22 +5099,22 @@
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="E85" s="3" t="s">
         <v>462</v>
       </c>
+      <c r="E85" s="5" t="s">
+        <v>463</v>
+      </c>
       <c r="F85" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -4968,22 +5131,22 @@
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="E86" s="3" t="s">
         <v>468</v>
       </c>
+      <c r="E86" s="5" t="s">
+        <v>469</v>
+      </c>
       <c r="F86" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
@@ -5000,22 +5163,22 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -5032,22 +5195,22 @@
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -5064,22 +5227,22 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>487</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -5096,22 +5259,22 @@
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
@@ -5128,22 +5291,22 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>499</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -5160,22 +5323,22 @@
     </row>
     <row r="92">
       <c r="A92" s="3" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
@@ -5192,22 +5355,22 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>511</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -5224,22 +5387,22 @@
     </row>
     <row r="94">
       <c r="A94" s="3" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -5256,22 +5419,22 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -5288,22 +5451,22 @@
     </row>
     <row r="96">
       <c r="A96" s="3" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E96" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>525</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -5320,22 +5483,22 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -5352,22 +5515,22 @@
     </row>
     <row r="98">
       <c r="A98" s="3" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
@@ -5384,22 +5547,22 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>457</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -5416,22 +5579,22 @@
     </row>
     <row r="100">
       <c r="A100" s="3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D100" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>546</v>
       </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
@@ -5448,22 +5611,22 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D101" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -5480,22 +5643,22 @@
     </row>
     <row r="102">
       <c r="A102" s="3" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
@@ -5512,22 +5675,22 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
@@ -5544,22 +5707,22 @@
     </row>
     <row r="104">
       <c r="A104" s="3" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
@@ -5576,22 +5739,22 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -5608,22 +5771,22 @@
     </row>
     <row r="106">
       <c r="A106" s="3" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
@@ -5640,22 +5803,22 @@
     </row>
     <row r="107">
       <c r="A107" s="2" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -5672,22 +5835,22 @@
     </row>
     <row r="108">
       <c r="A108" s="3" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
@@ -5704,22 +5867,22 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -5736,22 +5899,22 @@
     </row>
     <row r="110">
       <c r="A110" s="3" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
@@ -5768,22 +5931,22 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
@@ -5800,22 +5963,22 @@
     </row>
     <row r="112">
       <c r="A112" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>614</v>
+        <v>190</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
@@ -5832,22 +5995,22 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>617</v>
+        <v>195</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -6043,12 +6206,24 @@
       <c r="R119" s="2"/>
     </row>
     <row r="120">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
+      <c r="A120" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>658</v>
+      </c>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
@@ -6063,12 +6238,24 @@
       <c r="R120" s="3"/>
     </row>
     <row r="121">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
+      <c r="A121" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>661</v>
+      </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -6083,12 +6270,24 @@
       <c r="R121" s="2"/>
     </row>
     <row r="122">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
+      <c r="A122" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>669</v>
+      </c>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -6103,12 +6302,24 @@
       <c r="R122" s="3"/>
     </row>
     <row r="123">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
+      <c r="A123" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>675</v>
+      </c>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
@@ -6123,12 +6334,24 @@
       <c r="R123" s="2"/>
     </row>
     <row r="124">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
+      <c r="A124" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>681</v>
+      </c>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -6143,12 +6366,24 @@
       <c r="R124" s="3"/>
     </row>
     <row r="125">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
+      <c r="A125" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>687</v>
+      </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
@@ -6162,13 +6397,45 @@
       <c r="Q125" s="2"/>
       <c r="R125" s="2"/>
     </row>
+    <row r="126">
+      <c r="A126" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>693</v>
+      </c>
+    </row>
     <row r="127">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
+      <c r="A127" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>518</v>
+      </c>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -6183,12 +6450,24 @@
       <c r="R127" s="2"/>
     </row>
     <row r="128">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
+      <c r="A128" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>702</v>
+      </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>

</xml_diff>

<commit_message>
finish translations in student pages
</commit_message>
<xml_diff>
--- a/frontend/src/translations/TraduccionesMetahospital.xlsx
+++ b/frontend/src/translations/TraduccionesMetahospital.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="728">
   <si>
     <t>Tname</t>
   </si>
@@ -2132,6 +2132,69 @@
   </si>
   <si>
     <t>Ordua</t>
+  </si>
+  <si>
+    <t>show_filter</t>
+  </si>
+  <si>
+    <t>Show filter</t>
+  </si>
+  <si>
+    <t>Mostrar filtro</t>
+  </si>
+  <si>
+    <t>Erakutsi iragazkia</t>
+  </si>
+  <si>
+    <t>Mostra filtre</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Día</t>
+  </si>
+  <si>
+    <t>Eguna</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>hour_rage</t>
+  </si>
+  <si>
+    <t>Hour range</t>
+  </si>
+  <si>
+    <t>Rango de horas</t>
+  </si>
+  <si>
+    <t>Ordu tartea</t>
+  </si>
+  <si>
+    <t>Rang d'hores</t>
+  </si>
+  <si>
+    <t>Intervalo horario</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Filtrar</t>
+  </si>
+  <si>
+    <t>Iragazkia</t>
+  </si>
+  <si>
+    <t>Filtro</t>
   </si>
 </sst>
 </file>
@@ -6558,12 +6621,24 @@
       <c r="R130" s="3"/>
     </row>
     <row r="131">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
+      <c r="A131" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>709</v>
+      </c>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
@@ -6578,12 +6653,24 @@
       <c r="R131" s="2"/>
     </row>
     <row r="132">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
+      <c r="A132" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>714</v>
+      </c>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
@@ -6598,12 +6685,24 @@
       <c r="R132" s="3"/>
     </row>
     <row r="133">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
+      <c r="A133" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>722</v>
+      </c>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
@@ -6618,12 +6717,24 @@
       <c r="R133" s="2"/>
     </row>
     <row r="134">
-      <c r="A134" s="3"/>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
-      <c r="E134" s="3"/>
-      <c r="F134" s="3"/>
+      <c r="A134" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>727</v>
+      </c>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>

</xml_diff>

<commit_message>
finish translations in teacher pages
</commit_message>
<xml_diff>
--- a/frontend/src/translations/TraduccionesMetahospital.xlsx
+++ b/frontend/src/translations/TraduccionesMetahospital.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="757">
   <si>
     <t>Tname</t>
   </si>
@@ -2164,7 +2164,7 @@
     <t>Dia</t>
   </si>
   <si>
-    <t>hour_rage</t>
+    <t>hour_range</t>
   </si>
   <si>
     <t>Hour range</t>
@@ -2195,6 +2195,93 @@
   </si>
   <si>
     <t>Filtro</t>
+  </si>
+  <si>
+    <t>select_student</t>
+  </si>
+  <si>
+    <t>Selecciona un estudiante</t>
+  </si>
+  <si>
+    <t>Aukeratu ikasle bat</t>
+  </si>
+  <si>
+    <t>Selecciona un estudiant</t>
+  </si>
+  <si>
+    <t>Selecciona un alumno</t>
+  </si>
+  <si>
+    <t>successful_password_restart</t>
+  </si>
+  <si>
+    <t>Student password has been reset</t>
+  </si>
+  <si>
+    <t>La contraseña del estudiante ha sido reestablecida</t>
+  </si>
+  <si>
+    <t>Ikaslearen pasahitza berrezarri da</t>
+  </si>
+  <si>
+    <t>La contrasenya de l'estudiant ha estat restablida</t>
+  </si>
+  <si>
+    <t>Restableceuse o contrasinal do alumno</t>
+  </si>
+  <si>
+    <t>error_restarting_student_password</t>
+  </si>
+  <si>
+    <t>Error resetting student password</t>
+  </si>
+  <si>
+    <t>Error al restablecer la contraseña del estudiante</t>
+  </si>
+  <si>
+    <t>Errore bat gertatu da ikaslearen pasahitza berrezartzean</t>
+  </si>
+  <si>
+    <t>Error en restablir la contrasenya de l'estudiant</t>
+  </si>
+  <si>
+    <t>Produciuse un erro ao restablecer o contrasinal do alumno</t>
+  </si>
+  <si>
+    <t>student_grades</t>
+  </si>
+  <si>
+    <t>Student grades</t>
+  </si>
+  <si>
+    <t>Notas estudiantes</t>
+  </si>
+  <si>
+    <t>Ikasleen kalifikazioak</t>
+  </si>
+  <si>
+    <t>Qualificacions estudiants</t>
+  </si>
+  <si>
+    <t>Cualificacións dos estudantes</t>
+  </si>
+  <si>
+    <t>exercises_get_fail</t>
+  </si>
+  <si>
+    <t>Error getting exercises</t>
+  </si>
+  <si>
+    <t>Error al obtener ejercicios</t>
+  </si>
+  <si>
+    <t>Errore bat gertatu da ariketak eskuratzean</t>
+  </si>
+  <si>
+    <t>Error en obtenir exercicis</t>
+  </si>
+  <si>
+    <t>Erro ao conseguir exercicios</t>
   </si>
 </sst>
 </file>
@@ -6749,12 +6836,24 @@
       <c r="R134" s="3"/>
     </row>
     <row r="135">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2"/>
+      <c r="A135" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>732</v>
+      </c>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
@@ -6769,12 +6868,24 @@
       <c r="R135" s="2"/>
     </row>
     <row r="136">
-      <c r="A136" s="3"/>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
-      <c r="E136" s="3"/>
-      <c r="F136" s="3"/>
+      <c r="A136" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>738</v>
+      </c>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -6789,12 +6900,24 @@
       <c r="R136" s="3"/>
     </row>
     <row r="137">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
+      <c r="A137" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>744</v>
+      </c>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
@@ -6809,12 +6932,24 @@
       <c r="R137" s="2"/>
     </row>
     <row r="138">
-      <c r="A138" s="3"/>
-      <c r="B138" s="3"/>
-      <c r="C138" s="3"/>
-      <c r="D138" s="3"/>
-      <c r="E138" s="3"/>
-      <c r="F138" s="3"/>
+      <c r="A138" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>750</v>
+      </c>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
@@ -6829,12 +6964,24 @@
       <c r="R138" s="3"/>
     </row>
     <row r="139">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
+      <c r="A139" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>756</v>
+      </c>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
@@ -6849,8 +6996,6 @@
       <c r="R139" s="2"/>
     </row>
     <row r="140">
-      <c r="A140" s="3"/>
-      <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>

</xml_diff>

<commit_message>
add global view and download all grades excel
</commit_message>
<xml_diff>
--- a/frontend/src/translations/TraduccionesMetahospital.xlsx
+++ b/frontend/src/translations/TraduccionesMetahospital.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="806">
   <si>
     <t>Tname</t>
   </si>
@@ -2282,6 +2282,153 @@
   </si>
   <si>
     <t>Erro ao conseguir exercicios</t>
+  </si>
+  <si>
+    <t>final_grade</t>
+  </si>
+  <si>
+    <t>Final grade</t>
+  </si>
+  <si>
+    <t>Nota final</t>
+  </si>
+  <si>
+    <t>Azken nota</t>
+  </si>
+  <si>
+    <t>submit_date</t>
+  </si>
+  <si>
+    <t>Submit date</t>
+  </si>
+  <si>
+    <t>date_generated</t>
+  </si>
+  <si>
+    <t>Generation date</t>
+  </si>
+  <si>
+    <t>Fecha de generación</t>
+  </si>
+  <si>
+    <t>Sorkuntza data</t>
+  </si>
+  <si>
+    <t>Data de generació</t>
+  </si>
+  <si>
+    <t>Data de xeración</t>
+  </si>
+  <si>
+    <t>excel_general_student_information</t>
+  </si>
+  <si>
+    <t>General student information</t>
+  </si>
+  <si>
+    <t>Información general de los estudiantes</t>
+  </si>
+  <si>
+    <t>Ikasleen informazio orokorra</t>
+  </si>
+  <si>
+    <t>Informació general dels estudiants</t>
+  </si>
+  <si>
+    <t>Información xeral do alumnado</t>
+  </si>
+  <si>
+    <t>excel_general_information</t>
+  </si>
+  <si>
+    <t>General information</t>
+  </si>
+  <si>
+    <t>Información general</t>
+  </si>
+  <si>
+    <t>Informazio orokorra</t>
+  </si>
+  <si>
+    <t>Informació general</t>
+  </si>
+  <si>
+    <t>Información xeral</t>
+  </si>
+  <si>
+    <t>submit_time</t>
+  </si>
+  <si>
+    <t>Submit time</t>
+  </si>
+  <si>
+    <t>Hora de finalización</t>
+  </si>
+  <si>
+    <t>Bidalketa Ordua</t>
+  </si>
+  <si>
+    <t>Hora de finalització</t>
+  </si>
+  <si>
+    <t>Tempo de remate</t>
+  </si>
+  <si>
+    <t>global_view</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Globala</t>
+  </si>
+  <si>
+    <t>workUnit_view</t>
+  </si>
+  <si>
+    <t>Work Units</t>
+  </si>
+  <si>
+    <t>Unidades de trabajo</t>
+  </si>
+  <si>
+    <t>Lan-unitateak</t>
+  </si>
+  <si>
+    <t>Unitats de treball</t>
+  </si>
+  <si>
+    <t>Unidades de traballo</t>
+  </si>
+  <si>
+    <t>view_p</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Vista</t>
+  </si>
+  <si>
+    <t>Ikusi</t>
+  </si>
+  <si>
+    <t>Ver</t>
+  </si>
+  <si>
+    <t>view_s</t>
+  </si>
+  <si>
+    <t>Views</t>
+  </si>
+  <si>
+    <t>Vistas</t>
+  </si>
+  <si>
+    <t>Ikuspegiak</t>
+  </si>
+  <si>
+    <t>Vistes</t>
   </si>
 </sst>
 </file>
@@ -2575,7 +2722,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.13"/>
+    <col customWidth="1" min="1" max="1" width="26.88"/>
     <col customWidth="1" min="2" max="2" width="32.25"/>
     <col customWidth="1" min="3" max="3" width="29.75"/>
     <col customWidth="1" min="4" max="4" width="23.88"/>
@@ -6996,11 +7143,24 @@
       <c r="R139" s="2"/>
     </row>
     <row r="140">
-      <c r="C140" s="3"/>
-      <c r="D140" s="3"/>
-      <c r="E140" s="3"/>
-      <c r="F140" s="3"/>
-      <c r="G140" s="3"/>
+      <c r="A140" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>759</v>
+      </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
@@ -7014,12 +7174,24 @@
       <c r="R140" s="3"/>
     </row>
     <row r="141">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
+      <c r="A141" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
@@ -7034,12 +7206,24 @@
       <c r="R141" s="2"/>
     </row>
     <row r="142">
-      <c r="A142" s="3"/>
-      <c r="B142" s="3"/>
-      <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
-      <c r="E142" s="3"/>
-      <c r="F142" s="3"/>
+      <c r="A142" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>768</v>
+      </c>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
@@ -7054,12 +7238,24 @@
       <c r="R142" s="3"/>
     </row>
     <row r="143">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
+      <c r="A143" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>774</v>
+      </c>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
@@ -7074,12 +7270,24 @@
       <c r="R143" s="2"/>
     </row>
     <row r="144">
-      <c r="A144" s="3"/>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
+      <c r="A144" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>780</v>
+      </c>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
@@ -7094,12 +7302,24 @@
       <c r="R144" s="3"/>
     </row>
     <row r="145">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="F145" s="2"/>
+      <c r="A145" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>786</v>
+      </c>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
       <c r="I145" s="2"/>
@@ -7113,13 +7333,45 @@
       <c r="Q145" s="2"/>
       <c r="R145" s="2"/>
     </row>
+    <row r="146">
+      <c r="A146" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>788</v>
+      </c>
+    </row>
     <row r="147">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
+      <c r="A147" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>795</v>
+      </c>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
@@ -7134,12 +7386,24 @@
       <c r="R147" s="2"/>
     </row>
     <row r="148">
-      <c r="A148" s="3"/>
-      <c r="B148" s="3"/>
-      <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
-      <c r="F148" s="3"/>
+      <c r="A148" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>800</v>
+      </c>
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
@@ -7154,12 +7418,24 @@
       <c r="R148" s="3"/>
     </row>
     <row r="149">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
-      <c r="F149" s="2"/>
+      <c r="A149" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>803</v>
+      </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
@@ -7174,10 +7450,6 @@
       <c r="R149" s="2"/>
     </row>
     <row r="150">
-      <c r="A150" s="3"/>
-      <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
-      <c r="D150" s="3"/>
       <c r="E150" s="3"/>
       <c r="F150" s="3"/>
       <c r="G150" s="3"/>

</xml_diff>

<commit_message>
update translations, implement floatingExcelButton in groupGrades admin page and update viewsButton styles
</commit_message>
<xml_diff>
--- a/frontend/src/translations/TraduccionesMetahospital.xlsx
+++ b/frontend/src/translations/TraduccionesMetahospital.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="813">
   <si>
     <t>Tname</t>
   </si>
@@ -2429,6 +2429,27 @@
   </si>
   <si>
     <t>Vistes</t>
+  </si>
+  <si>
+    <t>Go Back</t>
+  </si>
+  <si>
+    <t>error_while_generating_excel</t>
+  </si>
+  <si>
+    <t>Error while generating excel</t>
+  </si>
+  <si>
+    <t>Error al generar excel</t>
+  </si>
+  <si>
+    <t>Errore bat gertatu da excel sortzean</t>
+  </si>
+  <si>
+    <t>Error en generar excel</t>
+  </si>
+  <si>
+    <t>Erro ao xerar Excel</t>
   </si>
 </sst>
 </file>
@@ -7450,8 +7471,24 @@
       <c r="R149" s="2"/>
     </row>
     <row r="150">
-      <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
+      <c r="A150" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>681</v>
+      </c>
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
@@ -7466,12 +7503,24 @@
       <c r="R150" s="3"/>
     </row>
     <row r="151">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
+      <c r="A151" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>812</v>
+      </c>
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
       <c r="I151" s="2"/>

</xml_diff>